<commit_message>
add data test case
</commit_message>
<xml_diff>
--- a/data/file.xlsx
+++ b/data/file.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="用户登录测试数据" sheetId="1" r:id="rId1"/>
+    <sheet name="参展宝展会测试数据" sheetId="2" r:id="rId2"/>
+    <sheet name="参展宝展装测试数据" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="77">
   <si>
     <t>观察员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,13 +40,293 @@
   </si>
   <si>
     <t>展装工厂</t>
+  </si>
+  <si>
+    <t>Test_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test_company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test_product</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test_city</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mobile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FromSite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FromSiteLocation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enterprise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainProduct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsFirstExhibit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntentCity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExhibitOn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RequireArea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntentExhibition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test_exhibit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Index_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home_Index_TopLeft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Exhibition_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//txzhanshang.zhankoo.com/Txzhanshang_Home_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//txzhanshang.zhankoo.com/Txzhanshang_Home_Detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Wiki_Home_Index_MiddleRight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Wiki_Home_Index_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Decorate_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-10-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9-18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19-36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37-54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55-72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73-108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109-200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试90761</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试意向城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试展品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ServiceItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExhibitionName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoothArea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinishOn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Budget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enterprise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home_Index_TopLeft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://help.zhankoo.com/Home_Index_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Index_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home_Index_MiddleRight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Exhibition_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Home_Decorate_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//exh.zhankoo.com_Decorate_DecorateCase_Detail_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//txzhanshang.zhankoo.com/Txzhanshang_Home_Detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Wiki_Home_Index_MiddleRight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//www.zhankoo.com_Wiki_Home_Index_BottomCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//txzhanshang.zhankoo.com/Txzhanshang_Home_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://help.zhankoo.com/Home_Index_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会展设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会展搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会展设计+搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-12-29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2万以下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2~3万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3~5万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5~8万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8~12万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12~18万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18~25万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25~30万</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30万以上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,13 +341,39 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,17 +385,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -388,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -402,68 +725,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1">
-        <v>13690769964</v>
-      </c>
-      <c r="B1" s="1">
-        <v>123456</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>13500000018</v>
+        <v>13690769964</v>
       </c>
       <c r="B2" s="1">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>18320836325</v>
+        <v>13500000018</v>
       </c>
       <c r="B3" s="1">
         <v>123456</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>18019237332</v>
+        <v>18320836325</v>
       </c>
       <c r="B4" s="1">
         <v>123456</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>18165702771</v>
+        <v>18019237332</v>
       </c>
       <c r="B5" s="1">
         <v>123456</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>18126127906</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>18165702771</v>
+      </c>
+      <c r="B6" s="1">
+        <v>123456</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>18126127906</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -476,26 +810,1126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.125" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="17.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>18126127906</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>18126127906</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>18126127906</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>18126127906</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>18126127906</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>18126127906</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>18126127906</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8">
+        <v>72</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>18126127906</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9">
+        <v>90</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>18126127906</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10">
+        <v>108</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>18126127906</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>18126127906</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>18126127906</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>18126127906</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>18126127906</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>18126127906</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>18126127906</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="8">
+        <v>200</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>18126127906</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="8">
+        <v>9</v>
+      </c>
+      <c r="K18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="J22" s="6"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="53.75" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="10.25" customWidth="1"/>
+    <col min="8" max="8" width="12.25" customWidth="1"/>
+    <col min="9" max="9" width="8.375" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>18126127906</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>18126127906</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>18126127906</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>18126127906</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>54</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>18126127906</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>75</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>18126127906</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>18126127906</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>18126127906</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9">
+        <v>220</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>18126127906</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>300</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>18126127906</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>18126127906</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>18</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>18126127906</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>27</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" display="http://exh.zhankoo.com/Home/DecorateBookInsert"/>
+    <hyperlink ref="D12" r:id="rId2"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>